<commit_message>
added date and automation status
SVN-Revision: 25428
</commit_message>
<xml_diff>
--- a/TestCases/ToBeAutomated/StorageType.xlsx
+++ b/TestCases/ToBeAutomated/StorageType.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18975" windowHeight="11955"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="17400" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
   <si>
     <t>Automated</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Test Case</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -122,12 +125,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -427,12 +433,15 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="53.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="53.28515625" style="1"/>
+    <col min="1" max="2" width="53.28515625" style="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="53.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
@@ -453,136 +462,238 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="45">
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="45">
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="45">
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="45">
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="45">
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="45">
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="45">
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="45">
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="45">
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="45">
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="45">
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="45">
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="45">
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="45">
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="45">
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="45">
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="20.25" customHeight="1">
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="3">
+        <v>40606</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="20.25" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -590,7 +701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="35.25" customHeight="1">
+    <row r="20" spans="1:4" ht="35.25" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>